<commit_message>
feat: curate carbohydrate as part of biomass equation
</commit_message>
<xml_diff>
--- a/ComplementaryData/biomass/biomassCalculations.xlsx
+++ b/ComplementaryData/biomass/biomassCalculations.xlsx
@@ -5,19 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\GitHub\hanpo-GEM\ComplementaryData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\GitHub\hanpo-GEM\ComplementaryData\biomass\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{999F2069-315D-4622-B362-115EEA0AAD69}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EC067EB-00F0-46D7-9F04-CA02136CDD11}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="27870" windowHeight="11010" xr2:uid="{6BD471C0-448F-42CA-B3A5-1BF336BA9B09}"/>
+    <workbookView xWindow="2790" yWindow="0" windowWidth="27870" windowHeight="11010" activeTab="1" xr2:uid="{6BD471C0-448F-42CA-B3A5-1BF336BA9B09}"/>
   </bookViews>
   <sheets>
     <sheet name="Calculations" sheetId="1" r:id="rId1"/>
     <sheet name="biomassCuration" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="solver_adj" localSheetId="0" hidden="1">Calculations!$F$54</definedName>
+    <definedName name="solver_adj" localSheetId="0" hidden="1">Calculations!$F$62</definedName>
     <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
     <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="1" hidden="1">1</definedName>
@@ -35,7 +35,7 @@
     <definedName name="solver_num" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_opt" localSheetId="1" hidden="1">biomassCuration!$G$58</definedName>
-    <definedName name="solver_opt" localSheetId="0" hidden="1">Calculations!$F$61</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">Calculations!$F$69</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
     <definedName name="solver_rbv" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="218">
   <si>
     <t>Nucleotide</t>
   </si>
@@ -673,6 +673,54 @@
   </si>
   <si>
     <t>Acyl chain</t>
+  </si>
+  <si>
+    <t>carbohydrate</t>
+  </si>
+  <si>
+    <t>glycogen</t>
+  </si>
+  <si>
+    <t>mannan</t>
+  </si>
+  <si>
+    <t>Carbohydrate</t>
+  </si>
+  <si>
+    <t>% of DCW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Taken from: </t>
+  </si>
+  <si>
+    <t>Table 5: take average of four strains; assume equal distribution across trehalose and glucans</t>
+  </si>
+  <si>
+    <t>(1-&gt;3)-beta-D-glucan</t>
+  </si>
+  <si>
+    <t>(1-&gt;6)-beta-D-glucan</t>
+  </si>
+  <si>
+    <t>trehalose</t>
+  </si>
+  <si>
+    <t>s_0001</t>
+  </si>
+  <si>
+    <t>s_0004</t>
+  </si>
+  <si>
+    <t>s_0773</t>
+  </si>
+  <si>
+    <t>s_1107</t>
+  </si>
+  <si>
+    <t>s_1520</t>
+  </si>
+  <si>
+    <t>s_3718</t>
   </si>
 </sst>
 </file>
@@ -820,7 +868,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -932,6 +980,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1247,10 +1298,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64F68CD7-9761-4C09-A414-4ADCA602E915}">
-  <dimension ref="A1:N66"/>
+  <dimension ref="A1:N74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E53" sqref="E53"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42:E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1334,6 +1385,7 @@
       <c r="G3" s="9" t="s">
         <v>45</v>
       </c>
+      <c r="J3" s="43"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="25" t="s">
@@ -1358,6 +1410,7 @@
         <f>0.003*(9.5/12)</f>
         <v>2.3749999999999999E-3</v>
       </c>
+      <c r="J4" s="43"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="25" t="s">
@@ -1381,6 +1434,7 @@
       <c r="G5" s="9" t="s">
         <v>42</v>
       </c>
+      <c r="J5" s="43"/>
     </row>
     <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="11"/>
@@ -1393,10 +1447,10 @@
         <f>G4/G2*1000</f>
         <v>7.2643453442457605E-3</v>
       </c>
-      <c r="J6" s="6"/>
+      <c r="J6" s="43"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J7" s="6"/>
+      <c r="J7" s="43"/>
     </row>
     <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J8" s="6"/>
@@ -2091,353 +2145,488 @@
       <c r="G39" s="33"/>
     </row>
     <row r="40" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="N40" s="30"/>
+      <c r="A40" s="33"/>
+      <c r="B40" s="33"/>
+      <c r="C40" s="33"/>
+      <c r="D40" s="33"/>
+      <c r="E40" s="33"/>
+      <c r="F40" s="33"/>
+      <c r="G40" s="33"/>
     </row>
     <row r="41" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="B41" s="19"/>
-      <c r="C41" s="19"/>
+      <c r="A41" s="20" t="s">
+        <v>207</v>
+      </c>
+      <c r="B41" s="18"/>
+      <c r="C41" s="18" t="s">
+        <v>208</v>
+      </c>
       <c r="D41" s="19"/>
-      <c r="E41" s="34"/>
-      <c r="F41" s="39"/>
-      <c r="G41" s="39"/>
+      <c r="E41" s="19"/>
+      <c r="N41" s="30"/>
     </row>
     <row r="42" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="20" t="s">
-        <v>200</v>
+      <c r="A42" s="1" t="s">
+        <v>205</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>58</v>
+        <v>206</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D42" s="20" t="s">
-        <v>196</v>
-      </c>
-      <c r="E42" s="40"/>
-      <c r="F42" s="40"/>
-      <c r="G42" s="40"/>
+      <c r="D42" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N42" s="30"/>
     </row>
     <row r="43" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="27" t="s">
-        <v>51</v>
-      </c>
-      <c r="B43" s="21">
-        <v>0.34</v>
-      </c>
-      <c r="C43" s="24">
-        <f t="shared" ref="C43:C48" si="5">B43/100</f>
-        <v>3.4000000000000002E-3</v>
-      </c>
-      <c r="D43" s="42"/>
-      <c r="E43" s="33"/>
-      <c r="F43" s="35"/>
-      <c r="G43" s="35"/>
+        <v>203</v>
+      </c>
+      <c r="B43" s="10">
+        <v>10.125</v>
+      </c>
+      <c r="C43" s="10">
+        <f>B43/100</f>
+        <v>0.10125000000000001</v>
+      </c>
+      <c r="D43" s="10">
+        <v>180.16</v>
+      </c>
+      <c r="E43" s="24">
+        <f>C43/D43*1000</f>
+        <v>0.56200044404973359</v>
+      </c>
+      <c r="N43" s="30"/>
     </row>
     <row r="44" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="27" t="s">
+        <v>204</v>
+      </c>
+      <c r="B44" s="10">
+        <v>35.325000000000003</v>
+      </c>
+      <c r="C44" s="10">
+        <f>B44/100</f>
+        <v>0.35325000000000001</v>
+      </c>
+      <c r="D44" s="10">
+        <v>180.16</v>
+      </c>
+      <c r="E44" s="24">
+        <f>C44/D44*1000</f>
+        <v>1.9607571047957373</v>
+      </c>
+      <c r="N44" s="30"/>
+    </row>
+    <row r="45" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="27" t="s">
+        <v>211</v>
+      </c>
+      <c r="B45" s="10">
+        <v>23.474999999999998</v>
+      </c>
+      <c r="C45" s="10">
+        <f>$B$45/3/100</f>
+        <v>7.8249999999999986E-2</v>
+      </c>
+      <c r="D45" s="10">
+        <v>342.29599999999999</v>
+      </c>
+      <c r="E45" s="24">
+        <f>C45/D45*1000</f>
+        <v>0.22860331409072845</v>
+      </c>
+      <c r="N45" s="30"/>
+    </row>
+    <row r="46" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="27" t="s">
+        <v>209</v>
+      </c>
+      <c r="B46" s="10"/>
+      <c r="C46" s="10">
+        <f>$B$45/3/100</f>
+        <v>7.8249999999999986E-2</v>
+      </c>
+      <c r="D46" s="10">
+        <v>180.16</v>
+      </c>
+      <c r="E46" s="24">
+        <f>C46/D46*1000</f>
+        <v>0.43433614564831252</v>
+      </c>
+      <c r="N46" s="30"/>
+    </row>
+    <row r="47" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="27" t="s">
+        <v>210</v>
+      </c>
+      <c r="B47" s="10"/>
+      <c r="C47" s="10">
+        <f>$B$45/3/100</f>
+        <v>7.8249999999999986E-2</v>
+      </c>
+      <c r="D47" s="10">
+        <v>180.16</v>
+      </c>
+      <c r="E47" s="24">
+        <f>C47/D47*1000</f>
+        <v>0.43433614564831252</v>
+      </c>
+      <c r="N47" s="30"/>
+    </row>
+    <row r="48" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N48" s="30"/>
+    </row>
+    <row r="49" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="B49" s="19"/>
+      <c r="C49" s="19"/>
+      <c r="D49" s="19"/>
+      <c r="E49" s="34"/>
+      <c r="F49" s="39"/>
+      <c r="G49" s="29"/>
+    </row>
+    <row r="50" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="20" t="s">
+        <v>200</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D50" s="20" t="s">
+        <v>196</v>
+      </c>
+      <c r="E50" s="40"/>
+      <c r="F50" s="40"/>
+      <c r="G50" s="40"/>
+    </row>
+    <row r="51" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="B51" s="21">
+        <v>0.34</v>
+      </c>
+      <c r="C51" s="24">
+        <f t="shared" ref="C51:C55" si="5">B51/100</f>
+        <v>3.4000000000000002E-3</v>
+      </c>
+      <c r="D51" s="42"/>
+      <c r="E51" s="33"/>
+      <c r="F51" s="35"/>
+      <c r="G51" s="35"/>
+    </row>
+    <row r="52" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="B44" s="21">
+      <c r="B52" s="21">
         <v>0.39</v>
       </c>
-      <c r="C44" s="24">
+      <c r="C52" s="24">
         <f t="shared" si="5"/>
         <v>3.9000000000000003E-3</v>
       </c>
-      <c r="D44" s="10"/>
-      <c r="E44" s="33"/>
-      <c r="F44" s="35"/>
-      <c r="G44" s="35"/>
-    </row>
-    <row r="45" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="27" t="s">
+      <c r="D52" s="10"/>
+      <c r="E52" s="33"/>
+      <c r="F52" s="35"/>
+      <c r="G52" s="35"/>
+    </row>
+    <row r="53" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="B45" s="21">
+      <c r="B53" s="21">
         <v>7.5999999999999998E-2</v>
       </c>
-      <c r="C45" s="24">
+      <c r="C53" s="24">
         <f t="shared" si="5"/>
         <v>7.5999999999999993E-4</v>
       </c>
-      <c r="D45" s="1" t="s">
+      <c r="D53" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="E45" s="33"/>
-      <c r="F45" s="35"/>
-      <c r="G45" s="35"/>
-    </row>
-    <row r="46" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="27" t="s">
+      <c r="E53" s="33"/>
+      <c r="F53" s="35"/>
+      <c r="G53" s="35"/>
+    </row>
+    <row r="54" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="B46" s="21">
+      <c r="B54" s="21">
         <v>0.45</v>
       </c>
-      <c r="C46" s="24">
+      <c r="C54" s="24">
         <f t="shared" si="5"/>
         <v>4.5000000000000005E-3</v>
       </c>
-      <c r="D46" s="10">
-        <f>SUM(C43:C50)</f>
+      <c r="D54" s="10">
+        <f>SUM(C51:C58)</f>
         <v>1.9960000000000002E-2</v>
       </c>
-      <c r="E46" s="33"/>
-      <c r="F46" s="35"/>
-      <c r="G46" s="35"/>
-    </row>
-    <row r="47" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="B47" s="21">
-        <v>0.35</v>
-      </c>
-      <c r="C47" s="24">
-        <f t="shared" si="5"/>
-        <v>3.4999999999999996E-3</v>
-      </c>
-      <c r="D47" s="10"/>
-      <c r="E47" s="33"/>
-      <c r="F47" s="35"/>
-      <c r="G47" s="35"/>
-    </row>
-    <row r="48" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="B48" s="21">
-        <v>0.39</v>
-      </c>
-      <c r="C48" s="10"/>
-      <c r="D48" s="10"/>
-      <c r="E48" s="33"/>
-      <c r="F48" s="35"/>
-      <c r="G48" s="35"/>
-    </row>
-    <row r="49" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="27" t="s">
-        <v>55</v>
-      </c>
-      <c r="B49" s="21"/>
-      <c r="C49" s="24">
-        <f>$B$48/2/100</f>
-        <v>1.9500000000000001E-3</v>
-      </c>
-      <c r="D49" s="10"/>
-      <c r="E49" s="33"/>
-      <c r="F49" s="35"/>
-      <c r="G49" s="35"/>
-    </row>
-    <row r="50" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="27" t="s">
-        <v>53</v>
-      </c>
-      <c r="B50" s="21"/>
-      <c r="C50" s="24">
-        <f>$B$48/2/100</f>
-        <v>1.9500000000000001E-3</v>
-      </c>
-      <c r="D50" s="10"/>
-      <c r="E50" s="33"/>
-      <c r="F50" s="35"/>
-      <c r="G50" s="35"/>
-    </row>
-    <row r="51" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="36"/>
-      <c r="B51" s="37"/>
-      <c r="C51" s="36"/>
-      <c r="D51" s="36"/>
-      <c r="E51" s="36"/>
-      <c r="F51" s="36"/>
-      <c r="G51" s="36"/>
-    </row>
-    <row r="52" spans="1:9" s="38" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="36"/>
-      <c r="B52" s="37"/>
-      <c r="C52" s="36"/>
-      <c r="D52" s="36"/>
-      <c r="E52" s="36"/>
-      <c r="F52" s="36"/>
-      <c r="G52" s="36"/>
-    </row>
-    <row r="53" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="E53" s="40"/>
-      <c r="F53" s="41"/>
-      <c r="G53" s="41"/>
-      <c r="H53" s="41"/>
-      <c r="I53" s="34"/>
-    </row>
-    <row r="54" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="B54" s="10">
-        <v>1.7</v>
-      </c>
-      <c r="C54" s="10"/>
-      <c r="D54" s="10"/>
       <c r="E54" s="33"/>
       <c r="F54" s="35"/>
       <c r="G54" s="35"/>
-      <c r="H54" s="34"/>
-      <c r="I54" s="34"/>
     </row>
     <row r="55" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="27" t="s">
-        <v>62</v>
-      </c>
-      <c r="B55" s="10">
-        <v>24.4</v>
-      </c>
-      <c r="C55" s="31">
-        <f>(100/SUM($B$55,$B$57:$B$59))*B55</f>
-        <v>25.765575501583953</v>
-      </c>
-      <c r="D55" s="24">
-        <f>(C55/100)*$D$46</f>
-        <v>5.1428088701161575E-3</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="B55" s="21">
+        <v>0.35</v>
+      </c>
+      <c r="C55" s="24">
+        <f t="shared" si="5"/>
+        <v>3.4999999999999996E-3</v>
+      </c>
+      <c r="D55" s="10"/>
       <c r="E55" s="33"/>
       <c r="F55" s="35"/>
       <c r="G55" s="35"/>
-      <c r="H55" s="34"/>
-      <c r="I55" s="34"/>
     </row>
     <row r="56" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="B56" s="10">
-        <v>3.5</v>
-      </c>
-      <c r="C56" s="32"/>
+        <v>60</v>
+      </c>
+      <c r="B56" s="21">
+        <v>0.39</v>
+      </c>
+      <c r="C56" s="10"/>
       <c r="D56" s="10"/>
       <c r="E56" s="33"/>
       <c r="F56" s="35"/>
       <c r="G56" s="35"/>
-      <c r="H56" s="34"/>
-      <c r="I56" s="34"/>
     </row>
     <row r="57" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="27" t="s">
-        <v>64</v>
-      </c>
-      <c r="B57" s="10">
-        <v>7.4</v>
-      </c>
-      <c r="C57" s="31">
-        <f>(100/SUM($B$55,$B$57:$B$59))*B57</f>
-        <v>7.8141499472016909</v>
-      </c>
-      <c r="D57" s="24">
-        <f>(C57/100)*$D$46</f>
-        <v>1.5597043294614578E-3</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="B57" s="21"/>
+      <c r="C57" s="24">
+        <f>$B$56/2/100</f>
+        <v>1.9500000000000001E-3</v>
+      </c>
+      <c r="D57" s="10"/>
       <c r="E57" s="33"/>
       <c r="F57" s="35"/>
       <c r="G57" s="35"/>
-      <c r="H57" s="34"/>
-      <c r="I57" s="34"/>
     </row>
     <row r="58" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="27" t="s">
-        <v>65</v>
-      </c>
-      <c r="B58" s="10">
-        <v>29.8</v>
-      </c>
-      <c r="C58" s="31">
-        <f>(100/SUM($B$55,$B$57:$B$59))*B58</f>
-        <v>31.467793030623024</v>
-      </c>
-      <c r="D58" s="24">
-        <f>(C58/100)*$D$46</f>
-        <v>6.2809714889123566E-3</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="B58" s="21"/>
+      <c r="C58" s="24">
+        <f>$B$56/2/100</f>
+        <v>1.9500000000000001E-3</v>
+      </c>
+      <c r="D58" s="10"/>
       <c r="E58" s="33"/>
       <c r="F58" s="35"/>
       <c r="G58" s="35"/>
-      <c r="H58" s="34"/>
-      <c r="I58" s="34"/>
-    </row>
-    <row r="59" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="27" t="s">
+    </row>
+    <row r="59" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="36"/>
+      <c r="B59" s="37"/>
+      <c r="C59" s="36"/>
+      <c r="D59" s="36"/>
+      <c r="E59" s="36"/>
+      <c r="F59" s="36"/>
+      <c r="G59" s="36"/>
+    </row>
+    <row r="60" spans="1:9" s="38" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="36"/>
+      <c r="B60" s="37"/>
+      <c r="C60" s="36"/>
+      <c r="D60" s="36"/>
+      <c r="E60" s="36"/>
+      <c r="F60" s="36"/>
+      <c r="G60" s="36"/>
+    </row>
+    <row r="61" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="E61" s="40"/>
+      <c r="F61" s="41"/>
+      <c r="G61" s="41"/>
+      <c r="H61" s="41"/>
+      <c r="I61" s="34"/>
+    </row>
+    <row r="62" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B62" s="10">
+        <v>1.7</v>
+      </c>
+      <c r="C62" s="10"/>
+      <c r="D62" s="10"/>
+      <c r="E62" s="33"/>
+      <c r="F62" s="35"/>
+      <c r="G62" s="35"/>
+      <c r="H62" s="34"/>
+      <c r="I62" s="34"/>
+    </row>
+    <row r="63" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="B63" s="10">
+        <v>24.4</v>
+      </c>
+      <c r="C63" s="31">
+        <f>(100/SUM($B$63,$B$65:$B$67))*B63</f>
+        <v>25.765575501583953</v>
+      </c>
+      <c r="D63" s="24">
+        <f>(C63/100)*$D$54</f>
+        <v>5.1428088701161575E-3</v>
+      </c>
+      <c r="E63" s="33"/>
+      <c r="F63" s="35"/>
+      <c r="G63" s="35"/>
+      <c r="H63" s="34"/>
+      <c r="I63" s="34"/>
+    </row>
+    <row r="64" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B64" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="C64" s="32"/>
+      <c r="D64" s="10"/>
+      <c r="E64" s="33"/>
+      <c r="F64" s="35"/>
+      <c r="G64" s="35"/>
+      <c r="H64" s="34"/>
+      <c r="I64" s="34"/>
+    </row>
+    <row r="65" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="B65" s="10">
+        <v>7.4</v>
+      </c>
+      <c r="C65" s="31">
+        <f>(100/SUM($B$63,$B$65:$B$67))*B65</f>
+        <v>7.8141499472016909</v>
+      </c>
+      <c r="D65" s="24">
+        <f>(C65/100)*$D$54</f>
+        <v>1.5597043294614578E-3</v>
+      </c>
+      <c r="E65" s="33"/>
+      <c r="F65" s="35"/>
+      <c r="G65" s="35"/>
+      <c r="H65" s="34"/>
+      <c r="I65" s="34"/>
+    </row>
+    <row r="66" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="B66" s="10">
+        <v>29.8</v>
+      </c>
+      <c r="C66" s="31">
+        <f>(100/SUM($B$63,$B$65:$B$67))*B66</f>
+        <v>31.467793030623024</v>
+      </c>
+      <c r="D66" s="24">
+        <f>(C66/100)*$D$54</f>
+        <v>6.2809714889123566E-3</v>
+      </c>
+      <c r="E66" s="33"/>
+      <c r="F66" s="35"/>
+      <c r="G66" s="35"/>
+      <c r="H66" s="34"/>
+      <c r="I66" s="34"/>
+    </row>
+    <row r="67" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="B59" s="10">
+      <c r="B67" s="10">
         <v>33.1</v>
       </c>
-      <c r="C59" s="31">
-        <f>(100/SUM($B$55,$B$57:$B$59))*B59</f>
+      <c r="C67" s="31">
+        <f>(100/SUM($B$63,$B$65:$B$67))*B67</f>
         <v>34.952481520591348</v>
       </c>
-      <c r="D59" s="24">
-        <f>(C59/100)*$D$46</f>
+      <c r="D67" s="24">
+        <f>(C67/100)*$D$54</f>
         <v>6.9765153115100339E-3</v>
       </c>
-      <c r="E59" s="33"/>
-      <c r="F59" s="35"/>
-      <c r="G59" s="35"/>
-    </row>
-    <row r="60" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="28" t="s">
+      <c r="E67" s="33"/>
+      <c r="F67" s="35"/>
+      <c r="G67" s="35"/>
+    </row>
+    <row r="68" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="B60" s="10">
+      <c r="B68" s="10">
         <v>0.1</v>
       </c>
-      <c r="C60" s="10"/>
-      <c r="D60" s="10"/>
-      <c r="E60" s="33"/>
-      <c r="F60" s="35"/>
-      <c r="G60" s="35"/>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A61" s="33"/>
-      <c r="B61" s="33"/>
-      <c r="C61" s="33"/>
-      <c r="D61" s="33"/>
-      <c r="E61" s="34"/>
-      <c r="F61" s="34"/>
-      <c r="G61" s="34"/>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A62" s="34"/>
-      <c r="B62" s="34"/>
-      <c r="C62" s="35"/>
-      <c r="D62" s="34"/>
-      <c r="E62" s="35"/>
-      <c r="F62" s="34"/>
-      <c r="G62" s="34"/>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G63"/>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G64"/>
-    </row>
-    <row r="65" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G65"/>
-    </row>
-    <row r="66" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G66"/>
+      <c r="C68" s="10"/>
+      <c r="D68" s="10"/>
+      <c r="E68" s="33"/>
+      <c r="F68" s="35"/>
+      <c r="G68" s="35"/>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A69" s="33"/>
+      <c r="B69" s="33"/>
+      <c r="C69" s="33"/>
+      <c r="D69" s="33"/>
+      <c r="E69" s="34"/>
+      <c r="F69" s="34"/>
+      <c r="G69" s="34"/>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A70" s="34"/>
+      <c r="B70" s="34"/>
+      <c r="C70" s="35"/>
+      <c r="D70" s="34"/>
+      <c r="E70" s="35"/>
+      <c r="F70" s="34"/>
+      <c r="G70" s="34"/>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G71"/>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G72"/>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G73"/>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G74"/>
     </row>
   </sheetData>
   <sortState ref="A18:F37">
@@ -2450,10 +2639,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37E04C23-51EF-41C3-AC01-2469F8FC9BA7}">
-  <dimension ref="A1:D65"/>
+  <dimension ref="A1:D71"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="D61" sqref="D61"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="D71" sqref="D71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3248,7 +3437,7 @@
         <v>103</v>
       </c>
       <c r="D53">
-        <f>-Calculations!C50</f>
+        <f>-Calculations!C58</f>
         <v>-1.9500000000000001E-3</v>
       </c>
     </row>
@@ -3263,7 +3452,7 @@
         <v>103</v>
       </c>
       <c r="D54">
-        <f>-Calculations!C47</f>
+        <f>-Calculations!C55</f>
         <v>-3.4999999999999996E-3</v>
       </c>
     </row>
@@ -3278,7 +3467,7 @@
         <v>103</v>
       </c>
       <c r="D55">
-        <f>-Calculations!C49</f>
+        <f>-Calculations!C57</f>
         <v>-1.9500000000000001E-3</v>
       </c>
     </row>
@@ -3293,7 +3482,7 @@
         <v>103</v>
       </c>
       <c r="D56">
-        <f>-Calculations!C46</f>
+        <f>-Calculations!C54</f>
         <v>-4.5000000000000005E-3</v>
       </c>
     </row>
@@ -3308,7 +3497,7 @@
         <v>103</v>
       </c>
       <c r="D57">
-        <f>-Calculations!C44</f>
+        <f>-Calculations!C52</f>
         <v>-3.9000000000000003E-3</v>
       </c>
     </row>
@@ -3323,7 +3512,7 @@
         <v>103</v>
       </c>
       <c r="D58">
-        <f>-Calculations!C43</f>
+        <f>-Calculations!C51</f>
         <v>-3.4000000000000002E-3</v>
       </c>
     </row>
@@ -3338,7 +3527,7 @@
         <v>103</v>
       </c>
       <c r="D59">
-        <f>-Calculations!C45</f>
+        <f>-Calculations!C53</f>
         <v>-7.5999999999999993E-4</v>
       </c>
     </row>
@@ -3367,7 +3556,7 @@
         <v>102</v>
       </c>
       <c r="D61">
-        <f>-Calculations!D55</f>
+        <f>-Calculations!D63</f>
         <v>-5.1428088701161575E-3</v>
       </c>
     </row>
@@ -3382,7 +3571,7 @@
         <v>102</v>
       </c>
       <c r="D62">
-        <f>-Calculations!D57</f>
+        <f>-Calculations!D65</f>
         <v>-1.5597043294614578E-3</v>
       </c>
     </row>
@@ -3397,7 +3586,7 @@
         <v>102</v>
       </c>
       <c r="D63">
-        <f>-Calculations!D58</f>
+        <f>-Calculations!D66</f>
         <v>-6.2809714889123566E-3</v>
       </c>
     </row>
@@ -3412,7 +3601,7 @@
         <v>102</v>
       </c>
       <c r="D64">
-        <f>-Calculations!D59</f>
+        <f>-Calculations!D67</f>
         <v>-6.9765153115100339E-3</v>
       </c>
     </row>
@@ -3427,6 +3616,100 @@
         <v>102</v>
       </c>
       <c r="D65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" t="str">
+        <f>Calculations!A43</f>
+        <v>glycogen</v>
+      </c>
+      <c r="B66" s="29" t="s">
+        <v>214</v>
+      </c>
+      <c r="C66" t="s">
+        <v>202</v>
+      </c>
+      <c r="D66">
+        <f>-Calculations!E43</f>
+        <v>-0.56200044404973359</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" t="str">
+        <f>Calculations!A44</f>
+        <v>mannan</v>
+      </c>
+      <c r="B67" s="29" t="s">
+        <v>215</v>
+      </c>
+      <c r="C67" t="s">
+        <v>202</v>
+      </c>
+      <c r="D67">
+        <f>-Calculations!E44</f>
+        <v>-1.9607571047957373</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" t="str">
+        <f>Calculations!A45</f>
+        <v>trehalose</v>
+      </c>
+      <c r="B68" s="29" t="s">
+        <v>216</v>
+      </c>
+      <c r="C68" t="s">
+        <v>202</v>
+      </c>
+      <c r="D68">
+        <f>-Calculations!E45</f>
+        <v>-0.22860331409072845</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" t="str">
+        <f>Calculations!A46</f>
+        <v>(1-&gt;3)-beta-D-glucan</v>
+      </c>
+      <c r="B69" t="s">
+        <v>212</v>
+      </c>
+      <c r="C69" t="s">
+        <v>202</v>
+      </c>
+      <c r="D69">
+        <f>-Calculations!E46</f>
+        <v>-0.43433614564831252</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" t="str">
+        <f>Calculations!A47</f>
+        <v>(1-&gt;6)-beta-D-glucan</v>
+      </c>
+      <c r="B70" t="s">
+        <v>213</v>
+      </c>
+      <c r="C70" t="s">
+        <v>202</v>
+      </c>
+      <c r="D70">
+        <f>-Calculations!E47</f>
+        <v>-0.43433614564831252</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>202</v>
+      </c>
+      <c r="B71" s="29" t="s">
+        <v>217</v>
+      </c>
+      <c r="C71" t="s">
+        <v>202</v>
+      </c>
+      <c r="D71">
         <v>1</v>
       </c>
     </row>

</xml_diff>